<commit_message>
Nuevas listas de coeficientes
</commit_message>
<xml_diff>
--- a/listas.xlsx
+++ b/listas.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python\Uptime_V4\trasteos varios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignasi.ferras\OneDrive - Dimension Data\_Dimension Data\_PACE 1.0\82 Uptime Commercials - anàlisi local FY2019\90 Configuración QT Fidel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D748B9-464E-4C73-B752-3C15556CB1B3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{B6E53ECF-E71E-4CDA-845F-2A5004843F87}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{34719881-AFB9-4AD3-A0D0-2DE6ADFC3202}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11565" xr2:uid="{3EAD9E70-DD07-4228-93AA-B0F3680493A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Trabajo" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="72">
   <si>
     <t>Servicio</t>
   </si>
@@ -66,9 +67,6 @@
     <t>COEF_LIST</t>
   </si>
   <si>
-    <t>ISM</t>
-  </si>
-  <si>
     <t>PSRU</t>
   </si>
   <si>
@@ -214,13 +212,49 @@
   </si>
   <si>
     <t>SUO1</t>
+  </si>
+  <si>
+    <t>PSBU</t>
+  </si>
+  <si>
+    <t>Cisco PSS Price List</t>
+  </si>
+  <si>
+    <t>SERVICE PROGRAM</t>
+  </si>
+  <si>
+    <t>File Name</t>
+  </si>
+  <si>
+    <t>Cisco UCS Price List</t>
+  </si>
+  <si>
+    <t>PARTNER SUPPORT SERVICES</t>
+  </si>
+  <si>
+    <t>UNIFIED COMPUTING SERVICES</t>
+  </si>
+  <si>
+    <t>SMART NET TOTAL CARE</t>
+  </si>
+  <si>
+    <t>CISCO SERVICES &amp; SUPPORT</t>
+  </si>
+  <si>
+    <t>Cisco SMT2 Price List</t>
+  </si>
+  <si>
+    <t>Cisco SMT3 Price List</t>
+  </si>
+  <si>
+    <t>Cisco SMT1 Price List</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -243,8 +277,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -263,6 +304,36 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD187D7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -277,7 +348,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -286,6 +357,38 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -293,6 +396,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFD187D7"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -604,7 +712,7 @@
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,25 +763,455 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="21">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="N2">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>28</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" s="21">
+        <v>6.3E-2</v>
+      </c>
+      <c r="N3">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I4" t="s">
+        <v>48</v>
+      </c>
+      <c r="L4" s="21">
+        <v>6.3E-2</v>
+      </c>
+      <c r="N4">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" t="s">
+        <v>45</v>
+      </c>
+      <c r="L5" s="21">
+        <v>6.3E-2</v>
+      </c>
+      <c r="N5">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" t="s">
+        <v>50</v>
+      </c>
+      <c r="L6" s="21">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="N6">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I7" t="s">
+        <v>53</v>
+      </c>
+      <c r="L7" s="21">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="N7">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8" t="s">
+        <v>55</v>
+      </c>
+      <c r="I8" t="s">
+        <v>56</v>
+      </c>
+      <c r="L8" s="21">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="N8">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H9" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9" t="s">
+        <v>59</v>
+      </c>
+      <c r="L9" s="21">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="N9">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" t="s">
+        <v>50</v>
+      </c>
+      <c r="L10" s="21">
+        <v>0.108</v>
+      </c>
+      <c r="N10">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" t="s">
+        <v>51</v>
+      </c>
+      <c r="H11" t="s">
+        <v>52</v>
+      </c>
+      <c r="I11" t="s">
+        <v>53</v>
+      </c>
+      <c r="L11" s="21">
+        <v>0.108</v>
+      </c>
+      <c r="N11">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H12" t="s">
+        <v>52</v>
+      </c>
+      <c r="I12" t="s">
+        <v>53</v>
+      </c>
+      <c r="L12" s="21">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="N12">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" t="s">
+        <v>54</v>
+      </c>
+      <c r="H13" t="s">
+        <v>55</v>
+      </c>
+      <c r="I13" t="s">
+        <v>56</v>
+      </c>
+      <c r="L13" s="21">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="N13">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="H14" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="L14" s="21">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="N14">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" t="s">
+        <v>57</v>
+      </c>
+      <c r="H15" t="s">
+        <v>58</v>
+      </c>
+      <c r="I15" t="s">
+        <v>59</v>
+      </c>
+      <c r="L15" s="21">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="N15">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02FD0E0F-A80C-42E2-90B8-921894178199}">
+  <dimension ref="A1:N23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="47.42578125" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="3"/>
+    <col min="11" max="11" width="9.140625" style="3"/>
+    <col min="13" max="13" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2"/>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="2"/>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="2"/>
+      <c r="N1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" t="s">
-        <v>40</v>
+      <c r="G2" s="12" t="s">
+        <v>39</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L2">
         <v>4.2000000000000003E-2</v>
@@ -684,25 +1222,25 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="G3" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" s="12" t="s">
         <v>42</v>
-      </c>
-      <c r="I3" t="s">
-        <v>43</v>
       </c>
       <c r="L3">
         <v>6.6000000000000003E-2</v>
@@ -713,25 +1251,25 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="G4" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" s="12" t="s">
         <v>48</v>
-      </c>
-      <c r="I4" t="s">
-        <v>49</v>
       </c>
       <c r="L4">
         <v>6.6000000000000003E-2</v>
@@ -742,25 +1280,25 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="G5" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" s="12" t="s">
         <v>45</v>
-      </c>
-      <c r="I5" t="s">
-        <v>46</v>
       </c>
       <c r="L5">
         <v>6.6000000000000003E-2</v>
@@ -771,19 +1309,19 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="G6" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" s="14" t="s">
         <v>50</v>
-      </c>
-      <c r="H6" t="s">
-        <v>51</v>
       </c>
       <c r="L6">
         <v>7.0000000000000007E-2</v>
@@ -794,25 +1332,25 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="G7" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" s="14" t="s">
         <v>53</v>
-      </c>
-      <c r="I7" t="s">
-        <v>54</v>
       </c>
       <c r="L7">
         <v>7.0000000000000007E-2</v>
@@ -823,25 +1361,25 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="G8" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" s="14" t="s">
         <v>56</v>
-      </c>
-      <c r="I8" t="s">
-        <v>57</v>
       </c>
       <c r="L8">
         <v>7.0000000000000007E-2</v>
@@ -852,25 +1390,25 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="G9" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="H9" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" s="14" t="s">
         <v>59</v>
-      </c>
-      <c r="I9" t="s">
-        <v>60</v>
       </c>
       <c r="L9">
         <v>7.0000000000000007E-2</v>
@@ -881,19 +1419,19 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="G10" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" s="12" t="s">
         <v>50</v>
-      </c>
-      <c r="H10" t="s">
-        <v>51</v>
       </c>
       <c r="L10">
         <v>0.12</v>
@@ -904,25 +1442,25 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="G11" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H11" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" s="14" t="s">
         <v>53</v>
-      </c>
-      <c r="I11" t="s">
-        <v>54</v>
       </c>
       <c r="L11">
         <v>0.12</v>
@@ -933,16 +1471,16 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H12" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" s="14" t="s">
         <v>53</v>
-      </c>
-      <c r="I12" t="s">
-        <v>54</v>
       </c>
       <c r="L12">
         <v>0.85</v>
@@ -953,16 +1491,16 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>27</v>
-      </c>
-      <c r="G13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="H13" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" s="14" t="s">
         <v>56</v>
-      </c>
-      <c r="I13" t="s">
-        <v>57</v>
       </c>
       <c r="L13">
         <v>0.85</v>
@@ -973,25 +1511,25 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G14" t="s">
+      <c r="G14" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H14" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" s="14" t="s">
         <v>53</v>
-      </c>
-      <c r="I14" t="s">
-        <v>54</v>
       </c>
       <c r="L14">
         <v>7.0000000000000007E-2</v>
@@ -1002,25 +1540,25 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D15" t="s">
-        <v>23</v>
-      </c>
-      <c r="G15" t="s">
+      <c r="G15" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="H15" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" s="14" t="s">
         <v>59</v>
-      </c>
-      <c r="I15" t="s">
-        <v>60</v>
       </c>
       <c r="L15">
         <v>0.08</v>
@@ -1029,8 +1567,81 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="6"/>
+    </row>
+    <row r="18" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+    </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>